<commit_message>
update code for Leave request
</commit_message>
<xml_diff>
--- a/Data/LeaveRequest_ESS_CZ_REG - Copy.xlsx
+++ b/Data/LeaveRequest_ESS_CZ_REG - Copy.xlsx
@@ -1,14 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A2937F-4C6D-41CA-9F4D-8F3457DE9C99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -83,26 +82,26 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
+      <color indexed="8"/>
+      <family val="2"/>
       <sz val="11"/>
-      <color indexed="8"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
+      <color indexed="29"/>
+      <family val="3"/>
       <sz val="11"/>
-      <color indexed="29"/>
       <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -139,6 +138,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
@@ -154,13 +160,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -439,14 +438,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0" zoomScale="110" zoomScaleNormal="110">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.35" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="49.54296875" customWidth="1"/>
@@ -459,7 +458,7 @@
     <col min="9" max="9" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -488,7 +487,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" ht="15.65" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10652573</v>
       </c>
@@ -517,7 +516,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" ht="15.65" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10652573</v>
       </c>
@@ -546,7 +545,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" ht="14.5" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10652573</v>
       </c>
@@ -575,7 +574,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" ht="14.5" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10652573</v>
       </c>
@@ -603,24 +602,24 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1 E3">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I5">
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="0"/>
 </worksheet>
 </file>
</xml_diff>